<commit_message>
Acabei de classificar toods os testes, só falta classificar o Treinamento
</commit_message>
<xml_diff>
--- a/Atividade_1/Spacex.xlsx
+++ b/Atividade_1/Spacex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\Jupyter\CD20-1\Atividade_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Estudo_CDados\Atividade_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CBA265-5683-4057-A4E6-C36C45022419}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E571DFA6-C346-48EC-92E9-F611C25DFBC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1426,12 +1426,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1773,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A125" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1823,1480 +1826,2130 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101" s="3"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110" s="3"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111" s="3"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" s="3"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" s="3"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" s="3"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" s="3"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" s="3"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" s="3"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" s="3"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119" s="3"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" s="3"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" s="3"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122" s="3"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123" s="3"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124" s="3"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125" s="3"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B132" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B133" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B134" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B135" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B136" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B137" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B138" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B139" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B140" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B141" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B142" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B143" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B144" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B145" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B146" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B147" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B148" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B149" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B150" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B151" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B152" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B153" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B154" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B155" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B156" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B157" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B158" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B159" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B160" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B161" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B162" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B163" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B164" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B165" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B166" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B167" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B168" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B169" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B170" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B171" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B172" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B173" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B174" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B175" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B176" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B177" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B178" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B179" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B180" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B181" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B182" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B183" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B184" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B185" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B186" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B187" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B188" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B189" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B190" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B191" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B192" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B193" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B194" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B195" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B196" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B197" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B198" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B199" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B200" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B201" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B202" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B203" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B204" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B205" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B206" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B207" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B208" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B209" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B210" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B211" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B212" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B213" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B214" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B215" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B216" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B217" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B218" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B219" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B220" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B221" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B222" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B223" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B224" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B225" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B226" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B227" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B228" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B229" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B230" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B231" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B232" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B233" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B234" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B235" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B236" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B237" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B238" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B239" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B240" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B241" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B242" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B243" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B244" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B245" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B246" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B247" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B248" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B249" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B250" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B251" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B252" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B253" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B254" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B255" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B256" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B257" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B258" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B259" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B260" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B261" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B262" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B263" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B264" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B265" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B266" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B267" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B268" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B269" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B270" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B271" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B272" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B273" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B274" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B275" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B276" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B277" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B278" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B279" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B280" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B281" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B282" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B283" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B284" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B285" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B286" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B287" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B288" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B289" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B290" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B291" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B292" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B293" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B294" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B295" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B296" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B297" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B298" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B299" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B300" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>300</v>
+      </c>
+      <c r="B301" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3309,450 +3962,716 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A88"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="255.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>388</v>
+      </c>
+      <c r="B88" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conclui agora o treinamento
</commit_message>
<xml_diff>
--- a/Atividade_1/Spacex.xlsx
+++ b/Atividade_1/Spacex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Estudo_CDados\Atividade_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E571DFA6-C346-48EC-92E9-F611C25DFBC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D415C632-0F59-4761-8B42-634DEB0D5617}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1776,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1789,12 +1789,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1802,7 +1803,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1810,7 +1811,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1818,8 +1819,8 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1834,715 +1835,953 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="3"/>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="3"/>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="3"/>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="3"/>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="3"/>
+      <c r="B50" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="3"/>
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="3"/>
+      <c r="B54" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="3"/>
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="3"/>
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="3"/>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="3"/>
+      <c r="B60" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="3"/>
+      <c r="B63" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="3"/>
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="3"/>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="3"/>
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="3"/>
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="3"/>
+      <c r="B68" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="3"/>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="3"/>
+      <c r="B70" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="3"/>
+      <c r="B71" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="3"/>
+      <c r="B72" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="3"/>
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="3"/>
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="3"/>
+      <c r="B75" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="3"/>
+      <c r="B76" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="3"/>
+      <c r="B77" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="3"/>
+      <c r="B78" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="3"/>
+      <c r="B79" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="3"/>
+      <c r="B80" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="3"/>
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="3"/>
+      <c r="B82" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="3"/>
+      <c r="B83" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="3"/>
+      <c r="B84" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="3"/>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="3"/>
+      <c r="B86" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="3"/>
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="3"/>
+      <c r="B88" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="3"/>
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="3"/>
+      <c r="B90" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="3"/>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="3"/>
+      <c r="B92" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="3"/>
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="3"/>
+      <c r="B94" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="3"/>
+      <c r="B95" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="3"/>
+      <c r="B96" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="3"/>
+      <c r="B97" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="3"/>
+      <c r="B98" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="3"/>
+      <c r="B99" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="3"/>
+      <c r="B100" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="3"/>
+      <c r="B101" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="3"/>
+      <c r="B102" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="3"/>
+      <c r="B103" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="3"/>
+      <c r="B104" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="3"/>
+      <c r="B105" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="3"/>
+      <c r="B106" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="3"/>
+      <c r="B107" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="3"/>
+      <c r="B108" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="3"/>
+      <c r="B109" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="3"/>
+      <c r="B110" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="3"/>
+      <c r="B111" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="3"/>
+      <c r="B112" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="3"/>
+      <c r="B113" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="3"/>
+      <c r="B114" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="3"/>
+      <c r="B115" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-      <c r="B116" s="3"/>
+      <c r="B116" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-      <c r="B117" s="3"/>
+      <c r="B117" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-      <c r="B118" s="3"/>
+      <c r="B118" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-      <c r="B119" s="3"/>
+      <c r="B119" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-      <c r="B120" s="3"/>
+      <c r="B120" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-      <c r="B121" s="3"/>
+      <c r="B121" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-      <c r="B122" s="3"/>
+      <c r="B122" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-      <c r="B123" s="3"/>
+      <c r="B123" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-      <c r="B124" s="3"/>
+      <c r="B124" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-      <c r="B125" s="3"/>
+      <c r="B125" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
@@ -3964,7 +4203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+    <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Terminado a limpeza dos tweets, naive_bayes é o próximo passo
</commit_message>
<xml_diff>
--- a/Atividade_1/Spacex.xlsx
+++ b/Atividade_1/Spacex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Estudo_CDados\Atividade_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D415C632-0F59-4761-8B42-634DEB0D5617}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11954446-F969-4639-81AB-5A66BF4B8E90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="390">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1357,6 +1357,9 @@
   </si>
   <si>
     <t>rt @schmitt_rosana: "luar no atlântico sul" #spaceart #moonproject #spaceflight #likeforfollowback #dearmoon #dearmoonproject #spacex  #elo…</t>
+  </si>
+  <si>
+    <t>qual</t>
   </si>
 </sst>
 </file>
@@ -1776,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="78" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView zoomScale="78" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1789,7 +1792,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4203,8 +4208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4216,6 +4221,9 @@
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
+      <c r="B1" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Finalizado a limpeza dos tweets, o próximo passo é o naive_bayes
</commit_message>
<xml_diff>
--- a/Atividade_1/Spacex.xlsx
+++ b/Atividade_1/Spacex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Estudo_CDados\Atividade_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11954446-F969-4639-81AB-5A66BF4B8E90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFA2120-B572-4238-8CE0-9E3B99A04E7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView zoomScale="78" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4208,8 +4208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Aqui o trabalho foi concluído com sucesso, note que algumas alterações foram feitas de uma vez. E que eu tive que dar uma boa organizada para não deixar poluído o diretório na hora da análise final
</commit_message>
<xml_diff>
--- a/Atividade_1/Spacex.xlsx
+++ b/Atividade_1/Spacex.xlsx
@@ -8,20 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Estudo_CDados\Atividade_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFA2120-B572-4238-8CE0-9E3B99A04E7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0360AFF4-FD55-4979-8041-A27918D1A740}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
     <sheet name="Teste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="388">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1072,14 +1080,6 @@
     <t>elon musk: faculdade não é importante".
 realidade: na lista de empregos abertos na spacex, praticamente nenhum cargo importante deixa de exigir pelo menos um bacharelado.
 https://t.co/xqk6mlqwgk</t>
-  </si>
-  <si>
-    <t>ué
-adiantaram???? https://t.co/lyn2bjwxvo</t>
-  </si>
-  <si>
-    <t>rt @anderbalm: cabe aos eua lançar uma missão até o tal asteroide alegando que a democracia está ameaçada por lá! 👌🏼
-https://t.co/4p6ebftc…</t>
   </si>
   <si>
     <t>rt @antoniocdff: aí sim vale a pena gastar todo ouro do mundo (principalmente do vaticano e inglaterra):
@@ -1779,7 +1779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="78" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="78" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4206,10 +4206,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="77" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4217,713 +4217,1034 @@
     <col min="1" max="1" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
       <c r="B1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>302</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>303</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>304</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>305</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="3">
+        <f t="shared" ref="C5:C68" si="0">C4 + 1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>306</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>307</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>308</v>
       </c>
       <c r="B8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>309</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>310</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>311</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>312</v>
       </c>
       <c r="B12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>313</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>314</v>
       </c>
       <c r="B14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>315</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>316</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>317</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>318</v>
       </c>
       <c r="B18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>319</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>320</v>
       </c>
       <c r="B20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>321</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>322</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>323</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>324</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>325</v>
       </c>
       <c r="B25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>326</v>
       </c>
       <c r="B26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>327</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>328</v>
       </c>
       <c r="B28" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>329</v>
       </c>
       <c r="B29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>330</v>
       </c>
       <c r="B30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>331</v>
       </c>
       <c r="B31" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>332</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>333</v>
       </c>
       <c r="B33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>334</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>335</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>336</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>337</v>
       </c>
       <c r="B37" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="3">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>338</v>
       </c>
       <c r="B38" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>339</v>
       </c>
       <c r="B39" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="3">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>340</v>
       </c>
       <c r="B40" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>341</v>
       </c>
       <c r="B41" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>342</v>
       </c>
       <c r="B42" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>343</v>
       </c>
       <c r="B43" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>344</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>345</v>
       </c>
       <c r="B45" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>346</v>
       </c>
       <c r="B46" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>347</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>348</v>
       </c>
       <c r="B48" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>349</v>
       </c>
       <c r="B49" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="3">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>350</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>351</v>
       </c>
       <c r="B51" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>352</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" s="3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>353</v>
       </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" s="3">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>354</v>
       </c>
       <c r="B54" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" s="3">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>355</v>
       </c>
       <c r="B55" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" s="3">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>356</v>
       </c>
       <c r="B56" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>357</v>
       </c>
       <c r="B57" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>358</v>
       </c>
       <c r="B58" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" s="3">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>359</v>
       </c>
       <c r="B59" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>360</v>
       </c>
       <c r="B60" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" s="3">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>361</v>
       </c>
       <c r="B61" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>362</v>
       </c>
       <c r="B62" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C62" s="3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>363</v>
       </c>
       <c r="B63" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63" s="3">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>364</v>
       </c>
       <c r="B64" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C64" s="3">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>365</v>
       </c>
       <c r="B65" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>366</v>
       </c>
       <c r="B66" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C66" s="3">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>367</v>
       </c>
       <c r="B67" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" s="3">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>368</v>
       </c>
       <c r="B68" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C68" s="3">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>369</v>
       </c>
       <c r="B69" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C69" s="3">
+        <f t="shared" ref="C69:C87" si="1">C68 + 1</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>370</v>
       </c>
       <c r="B70" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70" s="3">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>371</v>
       </c>
       <c r="B71" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" s="3">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>372</v>
       </c>
       <c r="B72" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" s="3">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>373</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" s="3">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>374</v>
       </c>
       <c r="B74" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" s="3">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>375</v>
       </c>
       <c r="B75" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C75" s="3">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>376</v>
       </c>
       <c r="B76" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" s="3">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>377</v>
       </c>
       <c r="B77" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77" s="3">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>378</v>
       </c>
       <c r="B78" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C78" s="3">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>379</v>
       </c>
       <c r="B79" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C79" s="3">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>380</v>
       </c>
       <c r="B80" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80" s="3">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>381</v>
       </c>
       <c r="B81" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C81" s="3">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>382</v>
       </c>
       <c r="B82" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>383</v>
       </c>
       <c r="B83" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83" s="3">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>384</v>
       </c>
       <c r="B84" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="C84" s="3">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>385</v>
       </c>
       <c r="B85" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C85" s="3">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>386</v>
       </c>
       <c r="B86" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>387</v>
-      </c>
-      <c r="B87" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>388</v>
-      </c>
-      <c r="B88" s="3">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="C86" s="3">
+        <f t="shared" si="1"/>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A17" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A15" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>